<commit_message>
Committing new tests from Q2 search and changes made in the existing files.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Check_ThatUserCanSearchByAnAlreadyExist_GF_Name.xlsx
+++ b/src/main/resources/testdata/Check_ThatUserCanSearchByAnAlreadyExist_GF_Name.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1125" windowWidth="13305" windowHeight="5790"/>
+    <workbookView xWindow="0" yWindow="1125" windowWidth="12720" windowHeight="5370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,6 @@
     <t>existingGF</t>
   </si>
   <si>
-    <t>selenium_GF1</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 test</t>
   </si>
@@ -45,6 +42,9 @@
   </si>
   <si>
     <t>check that user can search by an already exist GF &gt;&gt; Name</t>
+  </si>
+  <si>
+    <t>Name_AlreadyExist_Search</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +427,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -435,16 +435,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>